<commit_message>
Identificators per subject added. Now the message will sent valuable information about changes made.
</commit_message>
<xml_diff>
--- a/data_export.xlsx
+++ b/data_export.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zullo\OneDrive\Escritorio\Proyectos\College - Web Scrapping\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947BF469-98BB-4F62-BEEB-CA83A85983D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="New" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -94,7 +88,7 @@
     <t>94</t>
   </si>
   <si>
-    <t>Redes de Computadoras</t>
+    <t>Redes de Computadora</t>
   </si>
   <si>
     <t>97</t>
@@ -112,8 +106,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,21 +144,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -202,7 +188,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -236,7 +222,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -271,10 +256,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -447,17 +431,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -498,7 +479,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -539,7 +520,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -580,7 +561,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -621,7 +602,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -662,7 +643,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -703,7 +684,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -744,7 +725,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>28</v>
       </c>

</xml_diff>